<commit_message>
Updated data with most recent data
</commit_message>
<xml_diff>
--- a/Data/Wealth1percent.xlsx
+++ b/Data/Wealth1percent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/jo585802_ucf_edu/Documents/Documents/GitHub/ECO6416/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5E4746-99CC-0742-B5FB-32E85E7BA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FA5E4746-99CC-0742-B5FB-32E85E7BA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C286411B-F8BA-459D-85D8-40C2C72BD121}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -349,13 +349,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -366,7 +368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>32690</v>
       </c>
@@ -377,7 +379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>32782</v>
       </c>
@@ -388,7 +390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>32874</v>
       </c>
@@ -399,7 +401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>32964</v>
       </c>
@@ -410,7 +412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>33055</v>
       </c>
@@ -421,7 +423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>33147</v>
       </c>
@@ -432,7 +434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>33239</v>
       </c>
@@ -443,7 +445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>33329</v>
       </c>
@@ -454,7 +456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>33420</v>
       </c>
@@ -465,7 +467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>33512</v>
       </c>
@@ -476,7 +478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>33604</v>
       </c>
@@ -487,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>33695</v>
       </c>
@@ -498,7 +500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>33786</v>
       </c>
@@ -509,7 +511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>33878</v>
       </c>
@@ -520,7 +522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>33970</v>
       </c>
@@ -531,7 +533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>34060</v>
       </c>
@@ -542,7 +544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>34151</v>
       </c>
@@ -553,7 +555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>34243</v>
       </c>
@@ -564,7 +566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>34335</v>
       </c>
@@ -575,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>34425</v>
       </c>
@@ -586,7 +588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>34516</v>
       </c>
@@ -597,7 +599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>34608</v>
       </c>
@@ -608,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>34700</v>
       </c>
@@ -619,7 +621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>34790</v>
       </c>
@@ -630,7 +632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>34881</v>
       </c>
@@ -641,7 +643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>34973</v>
       </c>
@@ -652,7 +654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>35065</v>
       </c>
@@ -663,7 +665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>35156</v>
       </c>
@@ -674,7 +676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>35247</v>
       </c>
@@ -685,7 +687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>35339</v>
       </c>
@@ -696,7 +698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>35431</v>
       </c>
@@ -707,7 +709,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>35521</v>
       </c>
@@ -718,7 +720,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>35612</v>
       </c>
@@ -729,7 +731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>35704</v>
       </c>
@@ -740,7 +742,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35796</v>
       </c>
@@ -751,7 +753,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35886</v>
       </c>
@@ -762,7 +764,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35977</v>
       </c>
@@ -773,7 +775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>36069</v>
       </c>
@@ -784,7 +786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36161</v>
       </c>
@@ -795,7 +797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>36251</v>
       </c>
@@ -806,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>36342</v>
       </c>
@@ -817,7 +819,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>36434</v>
       </c>
@@ -828,7 +830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>36526</v>
       </c>
@@ -839,7 +841,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>36617</v>
       </c>
@@ -850,7 +852,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>36708</v>
       </c>
@@ -861,7 +863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>36800</v>
       </c>
@@ -872,7 +874,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>36892</v>
       </c>
@@ -883,7 +885,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>36982</v>
       </c>
@@ -894,7 +896,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>37073</v>
       </c>
@@ -905,7 +907,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>37165</v>
       </c>
@@ -916,7 +918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>37257</v>
       </c>
@@ -927,7 +929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>37347</v>
       </c>
@@ -938,7 +940,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>37438</v>
       </c>
@@ -949,7 +951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>37530</v>
       </c>
@@ -960,7 +962,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>37622</v>
       </c>
@@ -971,7 +973,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>37712</v>
       </c>
@@ -982,7 +984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>37803</v>
       </c>
@@ -993,7 +995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>37895</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>37987</v>
       </c>
@@ -1015,7 +1017,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>38078</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>38169</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>38261</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>38353</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>38443</v>
       </c>
@@ -1070,7 +1072,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>38534</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>38626</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>38718</v>
       </c>
@@ -1103,7 +1105,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>38808</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>38899</v>
       </c>
@@ -1125,7 +1127,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>38991</v>
       </c>
@@ -1136,7 +1138,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>39083</v>
       </c>
@@ -1147,7 +1149,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>39173</v>
       </c>
@@ -1158,7 +1160,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>39264</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>39356</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>39448</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>39539</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>39630</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>39722</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>39814</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>39904</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39995</v>
       </c>
@@ -1257,7 +1259,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>40087</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>40179</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>40269</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>40360</v>
       </c>
@@ -1301,7 +1303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>40452</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>40544</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>40634</v>
       </c>
@@ -1334,7 +1336,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>40725</v>
       </c>
@@ -1345,7 +1347,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>40817</v>
       </c>
@@ -1356,7 +1358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>40909</v>
       </c>
@@ -1367,7 +1369,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>41000</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>41091</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>41183</v>
       </c>
@@ -1400,7 +1402,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41275</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>41365</v>
       </c>
@@ -1422,7 +1424,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>41456</v>
       </c>
@@ -1433,7 +1435,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>41548</v>
       </c>
@@ -1444,7 +1446,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>41640</v>
       </c>
@@ -1455,7 +1457,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>41730</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>41821</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>41913</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>42005</v>
       </c>
@@ -1499,7 +1501,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>42095</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>42186</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>42278</v>
       </c>
@@ -1532,7 +1534,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>42370</v>
       </c>
@@ -1543,7 +1545,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>42461</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>42552</v>
       </c>
@@ -1565,7 +1567,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>42644</v>
       </c>
@@ -1576,7 +1578,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>42736</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>42826</v>
       </c>
@@ -1598,7 +1600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>42917</v>
       </c>
@@ -1609,7 +1611,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43009</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>43101</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43191</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43282</v>
       </c>
@@ -1653,7 +1655,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>43374</v>
       </c>
@@ -1664,7 +1666,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43466</v>
       </c>
@@ -1675,7 +1677,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43556</v>
       </c>
@@ -1686,7 +1688,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43647</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43739</v>
       </c>
@@ -1708,7 +1710,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43831</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>43922</v>
       </c>
@@ -1730,7 +1732,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44013</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44105</v>
       </c>
@@ -1752,15 +1754,59 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44197</v>
       </c>
       <c r="B128" s="2">
-        <v>32.1</v>
+        <v>31.9</v>
       </c>
       <c r="C128">
         <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B129" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="C129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B130" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="C130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B131" s="2">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B132" s="2">
+        <v>31.9</v>
+      </c>
+      <c r="C132">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed space in column name
</commit_message>
<xml_diff>
--- a/Data/Wealth1percent.xlsx
+++ b/Data/Wealth1percent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/jo585802_ucf_edu/Documents/Documents/GitHub/ECO6416/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FA5E4746-99CC-0742-B5FB-32E85E7BA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C286411B-F8BA-459D-85D8-40C2C72BD121}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{FA5E4746-99CC-0742-B5FB-32E85E7BA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAECCE2E-AD37-4EAC-8C2C-7BA1DAAC0805}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Time Counter</t>
-  </si>
-  <si>
     <t>Share</t>
   </si>
   <si>
     <t>quarter</t>
+  </si>
+  <si>
+    <t>TimeCounter</t>
   </si>
 </sst>
 </file>
@@ -351,21 +351,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>